<commit_message>
an unsaved xls file
</commit_message>
<xml_diff>
--- a/DesignDocs/F1 运行栈结构.xlsx
+++ b/DesignDocs/F1 运行栈结构.xlsx
@@ -150,7 +150,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,6 +163,13 @@
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -186,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -197,6 +204,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -501,7 +509,7 @@
   <dimension ref="A2:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -598,7 +606,7 @@
       <c r="B10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D10" t="s">

</xml_diff>